<commit_message>
populating new columns on Template file
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity_Sum_v2.xlsx
+++ b/rx_PSC_RentalActivity_Sum_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1582B624-51D1-4415-8D79-472E3723A159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C97BA0-8811-4768-B90C-076D853CD4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Unit Type</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, U5:U{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=display.OccSqFt</t>
+  </si>
+  <si>
+    <t>&amp;=display.SqFtChange</t>
   </si>
 </sst>
 </file>
@@ -343,8 +349,8 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -677,7 +683,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -691,7 +697,7 @@
     <col min="11" max="11" width="9.7265625" customWidth="1"/>
     <col min="12" max="12" width="7.54296875" customWidth="1"/>
     <col min="13" max="14" width="7.81640625" customWidth="1"/>
-    <col min="15" max="15" width="27.90625" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
     <col min="16" max="17" width="7.81640625" customWidth="1"/>
     <col min="18" max="18" width="6.90625" customWidth="1"/>
     <col min="19" max="19" width="8.54296875" customWidth="1"/>
@@ -892,8 +898,12 @@
       <c r="O5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="P5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>